<commit_message>
Made it so new flashcards could be added to sets + minor file reorganisation
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Jokes.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Jokes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -41,13 +41,32 @@
   </si>
   <si>
     <t>answer text</t>
+  </si>
+  <si>
+    <t>2023-10-07 23:12:07 36_12_6534199</t>
+  </si>
+  <si>
+    <t>What do you call a cow with no legs?</t>
+  </si>
+  <si>
+    <t>Ground beef!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="12">
+  <numFmts count="22">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
@@ -120,7 +139,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C5"/>
@@ -183,6 +202,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added Controller page and different pages for flashcards learning by user settings (for developing)
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Jokes.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Jokes.xlsx
@@ -65,7 +65,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="26">
+  <numFmts count="33">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>

</xml_diff>

<commit_message>
fixed create flashcards button
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Jokes.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/Jokes.xlsx
@@ -65,7 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="39">
+  <numFmts count="41">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>

</xml_diff>